<commit_message>
by bag and fee of bag
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CICO.xlsx
+++ b/src/main/resources/input_excel_file/booking/CICO.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Booking_By_Bag_Player1" sheetId="1" r:id="rId1"/>
-    <sheet name="Check_In_Bag_Player2" sheetId="4" r:id="rId2"/>
-    <sheet name="Check_In_Bag_Player3" sheetId="5" r:id="rId3"/>
+    <sheet name="Fee_Of_Bag_Player1" sheetId="4" r:id="rId2"/>
+    <sheet name="Fee_Of_Bag_Bill_Player1" sheetId="5" r:id="rId3"/>
     <sheet name="Check_In_Bag_Player4" sheetId="6" r:id="rId4"/>
     <sheet name="Undo_Check_In" sheetId="3" r:id="rId5"/>
     <sheet name="Check_In_Ekyc" sheetId="2" r:id="rId6"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="148">
   <si>
     <t>tc_id</t>
   </si>
@@ -74,9 +74,18 @@
     <t>assert_guest_style</t>
   </si>
   <si>
+    <t>assert_agency_id</t>
+  </si>
+  <si>
+    <t>assert_check_in_time</t>
+  </si>
+  <si>
     <t>assert_flight_id</t>
   </si>
   <si>
+    <t>assert_buggy_id</t>
+  </si>
+  <si>
     <t>assert_init_type</t>
   </si>
   <si>
@@ -86,7 +95,7 @@
     <t>assert_size_list_service_items</t>
   </si>
   <si>
-    <t>BB_001</t>
+    <t>VST_BY_BAG_001</t>
   </si>
   <si>
     <t>VST_Kiểm tra thông tin booking của bag</t>
@@ -98,13 +107,19 @@
     <t>booking_by_bag_request.json</t>
   </si>
   <si>
-    <t>CHI-LINH</t>
-  </si>
-  <si>
-    <t>CHI-LINH-123</t>
-  </si>
-  <si>
-    <t>23/10/2025</t>
+    <t>{{CTX:PARTNER_UID}}</t>
+  </si>
+  <si>
+    <t>{{CTX:COURSE_UID}}</t>
+  </si>
+  <si>
+    <t>{{CTX:BAG_0}}</t>
+  </si>
+  <si>
+    <t>{{TODAY}}</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
   <si>
     <t>booking_by_bag_expect.json</t>
@@ -122,6 +137,123 @@
     <t>BOOKING</t>
   </si>
   <si>
+    <t>AG_BY_BAG_001</t>
+  </si>
+  <si>
+    <t>AG_Kiểm tra thông tin booking của bag</t>
+  </si>
+  <si>
+    <t>TRADITIONAL</t>
+  </si>
+  <si>
+    <t>5D</t>
+  </si>
+  <si>
+    <t>assert_total_bill.total</t>
+  </si>
+  <si>
+    <t>assert_agency_paid_all</t>
+  </si>
+  <si>
+    <t>assert_total_bill.agency_pay</t>
+  </si>
+  <si>
+    <t>assert_agency_player_pay</t>
+  </si>
+  <si>
+    <t>assert_agency_paid_discount</t>
+  </si>
+  <si>
+    <t>assert_mush_pay_info.mush_pay</t>
+  </si>
+  <si>
+    <t>assert_rounds[0].green_fee</t>
+  </si>
+  <si>
+    <t>assert_rounds[0].caddie_fee</t>
+  </si>
+  <si>
+    <t>assert_rounds[0].voucher_green_fee_amount</t>
+  </si>
+  <si>
+    <t>assert_rounds[0].voucher_caddie_fee_amount</t>
+  </si>
+  <si>
+    <t>assert_total_golf_fee.green_fee</t>
+  </si>
+  <si>
+    <t>assert_total_golf_fee.caddie_fee</t>
+  </si>
+  <si>
+    <t>assert_total_golf_fee.total</t>
+  </si>
+  <si>
+    <t>assert_total_item_fee</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.golf_fee</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.rental</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.tee_driving</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.pro_shop</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.restaurant</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.kiosk</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.mini_bar</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.other_fee</t>
+  </si>
+  <si>
+    <t>assert_total_service_fee.total</t>
+  </si>
+  <si>
+    <t>VST_FEE_OF_BAG_001</t>
+  </si>
+  <si>
+    <t>VST_Kiểm tra thông tin phí của bag khi add 2 item proshop</t>
+  </si>
+  <si>
+    <t>fee_of_bag_request.json</t>
+  </si>
+  <si>
+    <t>fee_of_bag_expect.json</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>AG_FEE_OF_BAG_001</t>
+  </si>
+  <si>
+    <t>AG_Kiểm tra thông tin phí của bag khi add 2 item proshop</t>
+  </si>
+  <si>
+    <t>is_calc_detail_tax_and_fee</t>
+  </si>
+  <si>
+    <t>VST_FEE_OF_BAG_BILL_001</t>
+  </si>
+  <si>
+    <t>fee_of_bag_bill_request.json</t>
+  </si>
+  <si>
+    <t>fee_of_bag_bill_expect.json</t>
+  </si>
+  <si>
+    <t>AG_FEE_OF_BAG_BILL_001</t>
+  </si>
+  <si>
     <t>cms_user</t>
   </si>
   <si>
@@ -209,16 +341,13 @@
     <t>is_change_voucher</t>
   </si>
   <si>
-    <t>assert_check_in_time</t>
-  </si>
-  <si>
     <t>assert_bag_status</t>
   </si>
   <si>
     <t>assert_bag</t>
   </si>
   <si>
-    <t>CI_PLAYER2_001</t>
+    <t>CI_PLAYER4_001</t>
   </si>
   <si>
     <t>VST_Kiểm tra check in bag</t>
@@ -230,28 +359,28 @@
     <t>{{CTX:USER_NAME}}</t>
   </si>
   <si>
-    <t>{{CTX:BOOKING_UID_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:HOLE_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:GUEST_STYLE_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:GUEST_STYLE_NAME_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:BOOKING_DATE_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:COURSE_TYPE_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:TEE_TYPE_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:CUSTOMER_NAME_1}}</t>
+    <t>{{CTX:BOOKING_UID_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:HOLE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:GUEST_STYLE_NAME_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:BOOKING_DATE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:COURSE_TYPE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:TEE_TYPE_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:CUSTOMER_NAME_3}}</t>
   </si>
   <si>
     <t>CMS</t>
@@ -266,40 +395,37 @@
     <t>[]</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>check_in_bag_expect.json</t>
   </si>
   <si>
     <t>WAITING</t>
   </si>
   <si>
-    <t>CI_PLAYER2_002</t>
+    <t>CI_PLAYER4_002</t>
   </si>
   <si>
     <t>MB_Kiểm tra check in bag</t>
   </si>
   <si>
-    <t>{{CTX:MEMBER_UID_OF_GUEST_1}}</t>
-  </si>
-  <si>
-    <t>{{CTX:MEMBER_CARD_UID_1}}</t>
-  </si>
-  <si>
-    <t>CI_PLAYER2_003</t>
+    <t>{{CTX:MEMBER_UID_OF_GUEST_3}}</t>
+  </si>
+  <si>
+    <t>{{CTX:MEMBER_CARD_UID_3}}</t>
+  </si>
+  <si>
+    <t>CI_PLAYER4_003</t>
   </si>
   <si>
     <t>MBG_Kiểm tra check in bag</t>
   </si>
   <si>
-    <t>CI_PLAYER2_004</t>
+    <t>CI_PLAYER4_004</t>
   </si>
   <si>
     <t>NG_Kiểm tra check in bag</t>
   </si>
   <si>
-    <t>CI_PLAYER2_005</t>
+    <t>CI_PLAYER4_005</t>
   </si>
   <si>
     <t>AG_Kiểm tra check in bag</t>
@@ -311,96 +437,6 @@
     <t>true</t>
   </si>
   <si>
-    <t>CI_PLAYER3_001</t>
-  </si>
-  <si>
-    <t>{{CTX:BOOKING_UID_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:HOLE_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:GUEST_STYLE_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:GUEST_STYLE_NAME_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:BOOKING_DATE_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:COURSE_TYPE_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:TEE_TYPE_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:CUSTOMER_NAME_2}}</t>
-  </si>
-  <si>
-    <t>CI_PLAYER3_002</t>
-  </si>
-  <si>
-    <t>{{CTX:MEMBER_UID_OF_GUEST_2}}</t>
-  </si>
-  <si>
-    <t>{{CTX:MEMBER_CARD_UID_2}}</t>
-  </si>
-  <si>
-    <t>CI_PLAYER3_003</t>
-  </si>
-  <si>
-    <t>CI_PLAYER3_004</t>
-  </si>
-  <si>
-    <t>CI_PLAYER3_005</t>
-  </si>
-  <si>
-    <t>CI_PLAYER4_001</t>
-  </si>
-  <si>
-    <t>{{CTX:BOOKING_UID_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:HOLE_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:GUEST_STYLE_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:GUEST_STYLE_NAME_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:BOOKING_DATE_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:COURSE_TYPE_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:TEE_TYPE_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:CUSTOMER_NAME_3}}</t>
-  </si>
-  <si>
-    <t>CI_PLAYER4_002</t>
-  </si>
-  <si>
-    <t>{{CTX:MEMBER_UID_OF_GUEST_3}}</t>
-  </si>
-  <si>
-    <t>{{CTX:MEMBER_CARD_UID_3}}</t>
-  </si>
-  <si>
-    <t>CI_PLAYER4_003</t>
-  </si>
-  <si>
-    <t>CI_PLAYER4_004</t>
-  </si>
-  <si>
-    <t>CI_PLAYER4_005</t>
-  </si>
-  <si>
     <t>UCI_001</t>
   </si>
   <si>
@@ -432,15 +468,6 @@
   </si>
   <si>
     <t>{{CHECKSUM}}</t>
-  </si>
-  <si>
-    <t>{{CTX:PARTNER_UID}}</t>
-  </si>
-  <si>
-    <t>{{CTX:COURSE_UID}}</t>
-  </si>
-  <si>
-    <t>{{TODAY}}</t>
   </si>
   <si>
     <t>check_in_ekyc_expect.json</t>
@@ -644,7 +671,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,6 +699,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1009,7 +1048,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1033,16 +1072,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1051,89 +1090,89 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1194,16 +1233,40 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1742,13 +1805,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="19.8571428571429" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.9333333333333" style="1" customWidth="1"/>
@@ -1756,22 +1819,23 @@
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3047619047619" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8380952380952" style="11" customWidth="1"/>
     <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.8571428571429" style="1" customWidth="1"/>
     <col min="13" max="13" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.8666666666667" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.1238095238095" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.14285714285714" style="1"/>
+    <col min="14" max="14" width="20.3238095238095" style="1" customWidth="1"/>
+    <col min="15" max="16" width="24.8666666666667" style="1" customWidth="1"/>
+    <col min="17" max="18" width="16.1238095238095" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7142857142857" style="1" customWidth="1"/>
+    <col min="21" max="21" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:17">
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:20">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1784,16 +1848,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="22" t="s">
@@ -1823,57 +1887,137 @@
       <c r="Q1" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:17">
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:20">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="23">
-        <v>300</v>
-      </c>
-      <c r="H2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="23">
-        <v>2</v>
+      <c r="E2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>28</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="K2" s="7">
         <v>200</v>
       </c>
       <c r="L2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="7">
+        <v>1</v>
+      </c>
+      <c r="T2" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:20">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="I3" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="7">
+      <c r="J3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="7">
+        <v>200</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="7">
+        <v>378</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="7">
         <v>1</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="T3" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1886,13 +2030,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.8571428571429" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.9333333333333" style="1" customWidth="1"/>
@@ -1900,37 +2044,34 @@
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3047619047619" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5714285714286" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.8380952380952" style="11" customWidth="1"/>
-    <col min="14" max="15" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.8380952380952" style="11" customWidth="1"/>
-    <col min="17" max="18" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="19" max="19" width="21.1428571428571" style="11" customWidth="1"/>
-    <col min="20" max="21" width="24.7142857142857" style="1" customWidth="1"/>
-    <col min="22" max="27" width="12.7714285714286" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7714285714286" style="11" customWidth="1"/>
-    <col min="29" max="30" width="12.7714285714286" style="1" customWidth="1"/>
-    <col min="31" max="33" width="12.7714285714286" style="11" customWidth="1"/>
-    <col min="34" max="34" width="12.7714285714286" style="1" customWidth="1"/>
-    <col min="35" max="35" width="12.7714285714286" style="11" customWidth="1"/>
-    <col min="36" max="36" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="37" max="37" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="38" max="38" width="20.8571428571429" style="1" customWidth="1"/>
-    <col min="39" max="39" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="40" max="40" width="10.7142857142857" style="1" customWidth="1"/>
-    <col min="41" max="41" width="9.14285714285714" style="1"/>
-    <col min="42" max="42" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="43" max="43" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="44" max="44" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.14285714285714" style="1"/>
+    <col min="9" max="9" width="17.8380952380952" style="11" customWidth="1"/>
+    <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.8571428571429" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.6857142857143" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.047619047619" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.2380952380952" style="11" customWidth="1"/>
+    <col min="16" max="17" width="29.2380952380952" style="1" customWidth="1"/>
+    <col min="18" max="19" width="24.8666666666667" style="1" customWidth="1"/>
+    <col min="20" max="20" width="25.7047619047619" style="1" customWidth="1"/>
+    <col min="21" max="21" width="41.8380952380952" style="1" customWidth="1"/>
+    <col min="22" max="22" width="42.6857142857143" style="1" customWidth="1"/>
+    <col min="23" max="23" width="30.5809523809524" style="1" customWidth="1"/>
+    <col min="24" max="24" width="30.4190476190476" style="1" customWidth="1"/>
+    <col min="25" max="25" width="25.3714285714286" style="1" customWidth="1"/>
+    <col min="26" max="27" width="32.4285714285714" style="1" customWidth="1"/>
+    <col min="28" max="28" width="31.2571428571429" style="1" customWidth="1"/>
+    <col min="29" max="30" width="28.2380952380952" style="1" customWidth="1"/>
+    <col min="31" max="31" width="32.0952380952381" style="1" customWidth="1"/>
+    <col min="32" max="32" width="28.2380952380952" style="1" customWidth="1"/>
+    <col min="33" max="35" width="27.047619047619" style="1" customWidth="1"/>
+    <col min="36" max="36" width="23.352380952381" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:40">
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:36">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1943,631 +2084,352 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="I1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="M1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="N1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="O1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="P1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="Q1" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="R1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="T1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="U1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="V1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="W1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="X1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="Y1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="Z1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AB1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AC1" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AD1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AE1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AF1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AG1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AH1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AI1" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AJ1" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A2" s="12" t="s">
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:36">
+      <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="K2" s="7">
+        <v>200</v>
+      </c>
+      <c r="L2" s="21">
+        <v>2400000</v>
+      </c>
+      <c r="M2" s="28">
+        <v>0</v>
+      </c>
+      <c r="N2" s="28">
+        <v>0</v>
+      </c>
+      <c r="O2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="14">
+      <c r="P2" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="21">
+        <v>2400000</v>
+      </c>
+      <c r="R2" s="21">
+        <v>1</v>
+      </c>
+      <c r="S2" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="T2" s="30">
+        <v>600000</v>
+      </c>
+      <c r="U2" s="30">
+        <v>0</v>
+      </c>
+      <c r="V2" s="30">
+        <v>0</v>
+      </c>
+      <c r="W2" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="X2" s="30">
+        <v>600000</v>
+      </c>
+      <c r="Y2" s="30">
+        <v>1600000</v>
+      </c>
+      <c r="Z2" s="30">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="30">
+        <v>800000</v>
+      </c>
+      <c r="AB2" s="30">
+        <v>1600000</v>
+      </c>
+      <c r="AC2" s="30">
+        <v>600000</v>
+      </c>
+      <c r="AD2" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="30">
+        <v>200000</v>
+      </c>
+      <c r="AF2" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="30">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:36">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="7">
         <v>200</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" s="14">
-        <v>0</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14">
-        <v>0</v>
-      </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI2" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ2" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK2" s="14">
-        <v>200</v>
-      </c>
-      <c r="AL2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN2" s="14">
-        <f>G2</f>
-        <v>200</v>
+      <c r="L3" s="21">
+        <v>2400000</v>
+      </c>
+      <c r="M3" s="28">
+        <v>2000000</v>
+      </c>
+      <c r="N3" s="28">
+        <v>2000000</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="21">
+        <v>400000</v>
+      </c>
+      <c r="R3" s="21">
+        <v>1</v>
+      </c>
+      <c r="S3" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="T3" s="30">
+        <v>600000</v>
+      </c>
+      <c r="U3" s="30">
+        <v>0</v>
+      </c>
+      <c r="V3" s="30">
+        <v>0</v>
+      </c>
+      <c r="W3" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="X3" s="30">
+        <v>600000</v>
+      </c>
+      <c r="Y3" s="30">
+        <v>1600000</v>
+      </c>
+      <c r="Z3" s="30">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="30">
+        <v>800000</v>
+      </c>
+      <c r="AB3" s="30">
+        <v>1600000</v>
+      </c>
+      <c r="AC3" s="30">
+        <v>600000</v>
+      </c>
+      <c r="AD3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="30">
+        <v>200000</v>
+      </c>
+      <c r="AF3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="30">
+        <v>2400000</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A3" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="14">
-        <f>G2+1</f>
-        <v>201</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="14">
-        <v>0</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="V3" s="14">
-        <v>0</v>
-      </c>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI3" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ3" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK3" s="14">
-        <v>200</v>
-      </c>
-      <c r="AL3" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM3" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN3" s="14">
-        <f>G3</f>
-        <v>201</v>
-      </c>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="9:15">
+      <c r="I4" s="11"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="11"/>
     </row>
-    <row r="4" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A4" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="14">
-        <f>G3+1</f>
-        <v>202</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="O4" s="14">
-        <v>0</v>
-      </c>
-      <c r="P4" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="T4" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14">
-        <v>0</v>
-      </c>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
-      <c r="AH4" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI4" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ4" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK4" s="14">
-        <v>200</v>
-      </c>
-      <c r="AL4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM4" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN4" s="14">
-        <f>G4</f>
-        <v>202</v>
-      </c>
+    <row r="5" s="1" customFormat="1" customHeight="1" spans="9:15">
+      <c r="I5" s="11"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="11"/>
     </row>
-    <row r="5" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A5" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="14">
-        <f>G4+1</f>
-        <v>203</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" s="14">
-        <v>0</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14">
-        <v>0</v>
-      </c>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI5" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ5" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK5" s="14">
-        <v>200</v>
-      </c>
-      <c r="AL5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM5" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN5" s="14">
-        <f>G5</f>
-        <v>203</v>
-      </c>
+    <row r="6" s="1" customFormat="1" customHeight="1" spans="9:15">
+      <c r="I6" s="11"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="11"/>
     </row>
-    <row r="6" s="10" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A6" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="14">
-        <f>G5+1</f>
-        <v>204</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="O6" s="14">
-        <v>0</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="R6" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S6" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14">
-        <v>378</v>
-      </c>
-      <c r="W6" s="14">
-        <v>1600000</v>
-      </c>
-      <c r="X6" s="14">
-        <v>400000</v>
-      </c>
-      <c r="Y6" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH6" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ6" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK6" s="14">
-        <v>200</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN6" s="14">
-        <f>G6</f>
-        <v>204</v>
-      </c>
+    <row r="10" customHeight="1" spans="12:12">
+      <c r="L10" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2578,13 +2440,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.8571428571429" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.9333333333333" style="1" customWidth="1"/>
@@ -2592,37 +2454,23 @@
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3047619047619" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5714285714286" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.8380952380952" style="11" customWidth="1"/>
-    <col min="14" max="15" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.8380952380952" style="11" customWidth="1"/>
-    <col min="17" max="18" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="19" max="19" width="21.1428571428571" style="11" customWidth="1"/>
-    <col min="20" max="21" width="24.7142857142857" style="1" customWidth="1"/>
-    <col min="22" max="27" width="12.7714285714286" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7714285714286" style="11" customWidth="1"/>
-    <col min="29" max="30" width="12.7714285714286" style="1" customWidth="1"/>
-    <col min="31" max="33" width="12.7714285714286" style="11" customWidth="1"/>
-    <col min="34" max="34" width="12.7714285714286" style="1" customWidth="1"/>
-    <col min="35" max="35" width="12.7714285714286" style="11" customWidth="1"/>
-    <col min="36" max="36" width="31.4285714285714" style="1" customWidth="1"/>
-    <col min="37" max="37" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="38" max="38" width="20.8571428571429" style="1" customWidth="1"/>
-    <col min="39" max="39" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="40" max="40" width="10.7142857142857" style="1" customWidth="1"/>
-    <col min="41" max="41" width="9.14285714285714" style="1"/>
-    <col min="42" max="42" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="43" max="43" width="17.7142857142857" style="1" customWidth="1"/>
-    <col min="44" max="44" width="17.4285714285714" style="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.14285714285714" style="1"/>
+    <col min="9" max="9" width="31.9238095238095" style="11" customWidth="1"/>
+    <col min="10" max="10" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6857142857143" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.2380952380952" style="11" customWidth="1"/>
+    <col min="14" max="15" width="29.2380952380952" style="1" customWidth="1"/>
+    <col min="16" max="17" width="24.8666666666667" style="1" customWidth="1"/>
+    <col min="18" max="18" width="25.7047619047619" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41.8380952380952" style="1" customWidth="1"/>
+    <col min="20" max="20" width="42.6857142857143" style="1" customWidth="1"/>
+    <col min="21" max="21" width="32.4285714285714" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:40">
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2635,631 +2483,212 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="I1" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="3" t="s">
+      <c r="M1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="N1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="O1" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="P1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="R1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="S1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="T1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI1" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN1" s="9" t="s">
-        <v>60</v>
+      <c r="U1" s="25" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:40">
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:21">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="7">
-        <v>300</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="O2" s="7">
-        <v>0</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7">
-        <v>0</v>
-      </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI2" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK2" s="7">
+        <v>70</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="L2" s="28">
+        <v>0</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="28">
+        <v>0</v>
+      </c>
+      <c r="O2" s="21">
+        <v>2400000</v>
+      </c>
+      <c r="P2" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="R2" s="30">
+        <v>600000</v>
+      </c>
+      <c r="S2" s="30">
+        <v>0</v>
+      </c>
+      <c r="T2" s="30">
+        <v>0</v>
+      </c>
+      <c r="U2" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:21">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AM2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN2" s="7">
-        <f>G2</f>
-        <v>300</v>
+      <c r="I3" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="7">
+        <v>200</v>
+      </c>
+      <c r="L3" s="28">
+        <v>2000000</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="28">
+        <v>0</v>
+      </c>
+      <c r="O3" s="21">
+        <v>400000</v>
+      </c>
+      <c r="P3" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="R3" s="30">
+        <v>600000</v>
+      </c>
+      <c r="S3" s="30">
+        <v>0</v>
+      </c>
+      <c r="T3" s="30">
+        <v>0</v>
+      </c>
+      <c r="U3" s="30">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="7">
-        <f>G2+1</f>
-        <v>301</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="V3" s="7">
-        <v>0</v>
-      </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
-      <c r="AH3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI3" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK3" s="7">
-        <v>200</v>
-      </c>
-      <c r="AL3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM3" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN3" s="7">
-        <f>G3</f>
-        <v>301</v>
-      </c>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="9:13">
+      <c r="I4" s="11"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="11"/>
     </row>
-    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A4" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="7">
-        <f>G3+1</f>
-        <v>302</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="O4" s="7">
-        <v>0</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7">
-        <v>0</v>
-      </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI4" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ4" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK4" s="7">
-        <v>200</v>
-      </c>
-      <c r="AL4" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM4" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN4" s="7">
-        <f>G4</f>
-        <v>302</v>
-      </c>
+    <row r="5" s="1" customFormat="1" customHeight="1" spans="9:13">
+      <c r="I5" s="11"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="11"/>
     </row>
-    <row r="5" s="1" customFormat="1" customHeight="1" spans="1:40">
-      <c r="A5" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="7">
-        <f>G4+1</f>
-        <v>303</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="O5" s="7">
-        <v>0</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7">
-        <v>0</v>
-      </c>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI5" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK5" s="7">
-        <v>200</v>
-      </c>
-      <c r="AL5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN5" s="7">
-        <f>G5</f>
-        <v>303</v>
-      </c>
+    <row r="6" s="1" customFormat="1" customHeight="1" spans="9:13">
+      <c r="I6" s="11"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="11"/>
     </row>
-    <row r="6" customHeight="1" spans="1:40">
-      <c r="A6" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="7">
-        <f>G5+1</f>
-        <v>304</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="O6" s="7">
-        <v>0</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7">
-        <v>378</v>
-      </c>
-      <c r="W6" s="7">
-        <v>1600000</v>
-      </c>
-      <c r="X6" s="7">
-        <v>400000</v>
-      </c>
-      <c r="Y6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK6" s="7">
-        <v>200</v>
-      </c>
-      <c r="AL6" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN6" s="7">
-        <f>G6</f>
-        <v>304</v>
-      </c>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="9:13">
+      <c r="I10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3328,97 +2757,97 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AB1" s="16" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="AD1" s="15" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="AF1" s="16" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="AG1" s="16" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="AI1" s="19" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="AJ1" s="8" t="s">
         <v>9</v>
@@ -3427,30 +2856,30 @@
         <v>10</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" s="10" customFormat="1" customHeight="1" spans="1:40">
       <c r="A2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>108</v>
@@ -3483,16 +2912,16 @@
         <v>0</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="T2" s="14"/>
       <c r="U2" s="14"/>
@@ -3511,22 +2940,22 @@
       <c r="AF2" s="18"/>
       <c r="AG2" s="18"/>
       <c r="AH2" s="14" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="AI2" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AJ2" s="12" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="AK2" s="14">
         <v>200</v>
       </c>
       <c r="AL2" s="14" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AM2" s="14" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="AN2" s="14">
         <f>G2</f>
@@ -3535,19 +2964,19 @@
     </row>
     <row r="3" s="10" customFormat="1" customHeight="1" spans="1:40">
       <c r="A3" s="12" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>108</v>
@@ -3581,22 +3010,22 @@
         <v>0</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="V3" s="14">
         <v>0</v>
@@ -3613,22 +3042,22 @@
       <c r="AF3" s="18"/>
       <c r="AG3" s="18"/>
       <c r="AH3" s="14" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="AI3" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AJ3" s="12" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="AK3" s="14">
         <v>200</v>
       </c>
       <c r="AL3" s="14" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AM3" s="14" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="AN3" s="14">
         <f>G3</f>
@@ -3637,19 +3066,19 @@
     </row>
     <row r="4" s="10" customFormat="1" customHeight="1" spans="1:40">
       <c r="A4" s="12" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>108</v>
@@ -3683,19 +3112,19 @@
         <v>0</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="U4" s="14"/>
       <c r="V4" s="14">
@@ -3713,22 +3142,22 @@
       <c r="AF4" s="18"/>
       <c r="AG4" s="18"/>
       <c r="AH4" s="14" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="AI4" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AJ4" s="12" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="AK4" s="14">
         <v>200</v>
       </c>
       <c r="AL4" s="14" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AM4" s="14" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="AN4" s="14">
         <f>G4</f>
@@ -3737,19 +3166,19 @@
     </row>
     <row r="5" s="10" customFormat="1" customHeight="1" spans="1:40">
       <c r="A5" s="12" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>108</v>
@@ -3783,16 +3212,16 @@
         <v>0</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
@@ -3811,22 +3240,22 @@
       <c r="AF5" s="18"/>
       <c r="AG5" s="18"/>
       <c r="AH5" s="14" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="AI5" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AJ5" s="12" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="AK5" s="14">
         <v>200</v>
       </c>
       <c r="AL5" s="14" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AM5" s="14" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="AN5" s="14">
         <f>G5</f>
@@ -3835,19 +3264,19 @@
     </row>
     <row r="6" s="10" customFormat="1" customHeight="1" spans="1:40">
       <c r="A6" s="12" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>108</v>
@@ -3881,16 +3310,16 @@
         <v>0</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
@@ -3913,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="18" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="AC6" s="14">
         <v>0</v>
@@ -3922,31 +3351,31 @@
         <v>0</v>
       </c>
       <c r="AE6" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AF6" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AG6" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AH6" s="14" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="AI6" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AJ6" s="12" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="AK6" s="14">
         <v>200</v>
       </c>
       <c r="AL6" s="14" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AM6" s="14" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="AN6" s="14">
         <f>G6</f>
@@ -3999,7 +3428,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -4013,25 +3442,25 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="H2" s="7">
         <v>200</v>
@@ -4086,7 +3515,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -4095,7 +3524,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -4107,51 +3536,51 @@
         <v>10</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="K2" s="7">
         <v>200</v>
       </c>
-      <c r="L2" s="24" t="s">
-        <v>137</v>
+      <c r="L2" s="32" t="s">
+        <v>146</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
voucher add and voucher remove
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/CICO.xlsx
+++ b/src/main/resources/input_excel_file/booking/CICO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="16" activeTab="21"/>
+    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Booking_By_Bag_Player1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="326">
   <si>
     <t>tc_id</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>{}</t>
+  </si>
+  <si>
+    <t>VST_FEE_OF_BAG_APPLY_VOUCHER_001</t>
+  </si>
+  <si>
+    <t>VST_Kiểm tra thông tin phí của bag khi apply voucher</t>
+  </si>
+  <si>
+    <t>VST_FEE_OF_BAG_APPLY_VOUCHER_002</t>
   </si>
   <si>
     <t>VST_BAG_SUB_001</t>
@@ -2711,7 +2720,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>9</v>
@@ -2755,7 +2764,7 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>66</v>
@@ -2780,7 +2789,7 @@
         <v>68</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K2" s="9">
         <v>200</v>
@@ -2819,7 +2828,7 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>70</v>
@@ -2844,7 +2853,7 @@
         <v>68</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K3" s="9">
         <v>200</v>
@@ -2883,7 +2892,7 @@
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A4" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>72</v>
@@ -2908,7 +2917,7 @@
         <v>68</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K4" s="9">
         <v>200</v>
@@ -2947,7 +2956,7 @@
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A5" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>72</v>
@@ -2972,7 +2981,7 @@
         <v>68</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K5" s="9">
         <v>200</v>
@@ -3013,7 +3022,7 @@
     </row>
     <row r="6" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A6" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>76</v>
@@ -3038,7 +3047,7 @@
         <v>68</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K6" s="9">
         <v>200</v>
@@ -3150,7 +3159,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>9</v>
@@ -3194,7 +3203,7 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>66</v>
@@ -3219,7 +3228,7 @@
         <v>68</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K2" s="9">
         <v>200</v>
@@ -3258,7 +3267,7 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>70</v>
@@ -3283,7 +3292,7 @@
         <v>68</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K3" s="9">
         <v>200</v>
@@ -3322,7 +3331,7 @@
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A4" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>72</v>
@@ -3347,7 +3356,7 @@
         <v>68</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K4" s="9">
         <v>200</v>
@@ -3386,7 +3395,7 @@
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A5" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>76</v>
@@ -3411,7 +3420,7 @@
         <v>68</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K5" s="9">
         <v>200</v>
@@ -3521,7 +3530,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>9</v>
@@ -3565,7 +3574,7 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>66</v>
@@ -3581,7 +3590,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>26</v>
@@ -3590,7 +3599,7 @@
         <v>68</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K2" s="9">
         <v>200</v>
@@ -3629,7 +3638,7 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>70</v>
@@ -3645,7 +3654,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>26</v>
@@ -3654,7 +3663,7 @@
         <v>68</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K3" s="9">
         <v>200</v>
@@ -3693,7 +3702,7 @@
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A4" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>72</v>
@@ -3709,7 +3718,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>26</v>
@@ -3718,7 +3727,7 @@
         <v>68</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K4" s="9">
         <v>200</v>
@@ -3757,7 +3766,7 @@
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:22">
       <c r="A5" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>76</v>
@@ -3773,7 +3782,7 @@
         <v>24</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>26</v>
@@ -3782,7 +3791,7 @@
         <v>68</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K5" s="9">
         <v>200</v>
@@ -3875,25 +3884,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="L1" s="27" t="s">
         <v>9</v>
@@ -3902,37 +3911,37 @@
         <v>10</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" s="29" customFormat="1" ht="166" customHeight="1" spans="1:14">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M2" s="14">
         <v>200</v>
@@ -3943,36 +3952,36 @@
     </row>
     <row r="3" s="29" customFormat="1" ht="166" customHeight="1" spans="1:14">
       <c r="A3" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M3" s="14">
         <v>200</v>
@@ -3983,40 +3992,40 @@
     </row>
     <row r="4" s="29" customFormat="1" ht="166" customHeight="1" spans="1:14">
       <c r="A4" s="6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C4" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>106</v>
-      </c>
       <c r="I4" s="14" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M4" s="14">
         <v>200</v>
@@ -4072,31 +4081,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="N1" s="27" t="s">
         <v>9</v>
@@ -4111,24 +4120,24 @@
         <v>43</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:19">
       <c r="A2" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>23</v>
@@ -4137,28 +4146,28 @@
         <v>24</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M2" s="28" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="O2" s="9">
         <v>200</v>
@@ -4240,76 +4249,76 @@
         <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="U1" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V1" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="W1" s="19" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="X1" s="25" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Z1" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AA1" s="25" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AC1" s="10" t="s">
         <v>9</v>
@@ -4321,24 +4330,24 @@
         <v>41</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A2" s="5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>23</v>
@@ -4347,28 +4356,28 @@
         <v>24</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>68</v>
@@ -4393,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y2" s="9">
         <v>0</v>
@@ -4408,7 +4417,7 @@
         <v>68</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD2" s="14">
         <v>200</v>
@@ -4422,19 +4431,19 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A3" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>23</v>
@@ -4443,28 +4452,28 @@
         <v>24</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>68</v>
@@ -4489,7 +4498,7 @@
         <v>400000</v>
       </c>
       <c r="X3" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y3" s="9">
         <v>0</v>
@@ -4504,7 +4513,7 @@
         <v>68</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD3" s="14">
         <v>200</v>
@@ -4518,19 +4527,19 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A4" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>23</v>
@@ -4539,28 +4548,28 @@
         <v>24</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="P4" s="24" t="s">
         <v>68</v>
@@ -4585,7 +4594,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y4" s="9">
         <v>0</v>
@@ -4600,7 +4609,7 @@
         <v>68</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD4" s="14">
         <v>200</v>
@@ -4614,19 +4623,19 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A5" s="5" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>23</v>
@@ -4635,28 +4644,28 @@
         <v>24</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="P5" s="24" t="s">
         <v>68</v>
@@ -4681,7 +4690,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y5" s="9">
         <v>0</v>
@@ -4696,7 +4705,7 @@
         <v>68</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD5" s="14">
         <v>200</v>
@@ -4710,19 +4719,19 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A6" s="5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>23</v>
@@ -4731,28 +4740,28 @@
         <v>24</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="P6" s="24" t="s">
         <v>68</v>
@@ -4777,7 +4786,7 @@
         <v>400000</v>
       </c>
       <c r="X6" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y6" s="9">
         <v>0</v>
@@ -4792,7 +4801,7 @@
         <v>68</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD6" s="14">
         <v>200</v>
@@ -4868,76 +4877,76 @@
         <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="U1" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V1" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="W1" s="19" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="X1" s="25" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Z1" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AA1" s="25" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AC1" s="10" t="s">
         <v>9</v>
@@ -4949,24 +4958,24 @@
         <v>41</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A2" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>23</v>
@@ -4975,28 +4984,28 @@
         <v>24</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>68</v>
@@ -5021,7 +5030,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y2" s="9">
         <v>0</v>
@@ -5036,7 +5045,7 @@
         <v>68</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD2" s="14">
         <v>200</v>
@@ -5050,19 +5059,19 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A3" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>23</v>
@@ -5071,28 +5080,28 @@
         <v>24</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>68</v>
@@ -5117,7 +5126,7 @@
         <v>400000</v>
       </c>
       <c r="X3" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y3" s="9">
         <v>0</v>
@@ -5132,7 +5141,7 @@
         <v>68</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD3" s="14">
         <v>200</v>
@@ -5146,19 +5155,19 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A4" s="5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>23</v>
@@ -5167,28 +5176,28 @@
         <v>24</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="P4" s="24" t="s">
         <v>68</v>
@@ -5213,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y4" s="9">
         <v>0</v>
@@ -5228,7 +5237,7 @@
         <v>68</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD4" s="14">
         <v>200</v>
@@ -5242,19 +5251,19 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A5" s="5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>23</v>
@@ -5263,28 +5272,28 @@
         <v>24</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="P5" s="24" t="s">
         <v>68</v>
@@ -5309,7 +5318,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y5" s="9">
         <v>0</v>
@@ -5324,7 +5333,7 @@
         <v>68</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD5" s="14">
         <v>200</v>
@@ -5338,19 +5347,19 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A6" s="5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>23</v>
@@ -5359,28 +5368,28 @@
         <v>24</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="P6" s="24" t="s">
         <v>68</v>
@@ -5405,7 +5414,7 @@
         <v>400000</v>
       </c>
       <c r="X6" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y6" s="9">
         <v>0</v>
@@ -5420,7 +5429,7 @@
         <v>68</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD6" s="14">
         <v>200</v>
@@ -5496,76 +5505,76 @@
         <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="U1" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V1" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="W1" s="19" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="X1" s="25" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Z1" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AA1" s="25" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AC1" s="10" t="s">
         <v>9</v>
@@ -5577,24 +5586,24 @@
         <v>41</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A2" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>23</v>
@@ -5603,28 +5612,28 @@
         <v>24</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>68</v>
@@ -5649,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y2" s="9">
         <v>0</v>
@@ -5664,7 +5673,7 @@
         <v>68</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD2" s="14">
         <v>200</v>
@@ -5678,19 +5687,19 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A3" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>23</v>
@@ -5699,28 +5708,28 @@
         <v>24</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>68</v>
@@ -5745,7 +5754,7 @@
         <v>400000</v>
       </c>
       <c r="X3" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y3" s="9">
         <v>0</v>
@@ -5760,7 +5769,7 @@
         <v>68</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD3" s="14">
         <v>200</v>
@@ -5774,19 +5783,19 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A4" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>23</v>
@@ -5795,28 +5804,28 @@
         <v>24</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P4" s="24" t="s">
         <v>68</v>
@@ -5841,7 +5850,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y4" s="9">
         <v>0</v>
@@ -5856,7 +5865,7 @@
         <v>68</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD4" s="14">
         <v>200</v>
@@ -5870,19 +5879,19 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A5" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>23</v>
@@ -5891,28 +5900,28 @@
         <v>24</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P5" s="24" t="s">
         <v>68</v>
@@ -5937,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y5" s="9">
         <v>0</v>
@@ -5952,7 +5961,7 @@
         <v>68</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD5" s="14">
         <v>200</v>
@@ -5966,19 +5975,19 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A6" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>23</v>
@@ -5987,28 +5996,28 @@
         <v>24</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P6" s="24" t="s">
         <v>68</v>
@@ -6033,7 +6042,7 @@
         <v>400000</v>
       </c>
       <c r="X6" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y6" s="9">
         <v>0</v>
@@ -6048,7 +6057,7 @@
         <v>68</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD6" s="14">
         <v>200</v>
@@ -6124,76 +6133,76 @@
         <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="U1" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V1" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="W1" s="19" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="X1" s="25" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Z1" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AA1" s="25" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AC1" s="10" t="s">
         <v>9</v>
@@ -6205,24 +6214,24 @@
         <v>41</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A2" s="5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>23</v>
@@ -6231,28 +6240,28 @@
         <v>24</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>68</v>
@@ -6277,7 +6286,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y2" s="9">
         <v>0</v>
@@ -6292,7 +6301,7 @@
         <v>68</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD2" s="14">
         <v>200</v>
@@ -6306,19 +6315,19 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A3" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>23</v>
@@ -6327,28 +6336,28 @@
         <v>24</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>68</v>
@@ -6373,7 +6382,7 @@
         <v>400000</v>
       </c>
       <c r="X3" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y3" s="9">
         <v>0</v>
@@ -6388,7 +6397,7 @@
         <v>68</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD3" s="14">
         <v>200</v>
@@ -6402,19 +6411,19 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A4" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>23</v>
@@ -6423,28 +6432,28 @@
         <v>24</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P4" s="24" t="s">
         <v>68</v>
@@ -6469,7 +6478,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y4" s="9">
         <v>0</v>
@@ -6484,7 +6493,7 @@
         <v>68</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD4" s="14">
         <v>200</v>
@@ -6498,19 +6507,19 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A5" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>23</v>
@@ -6519,28 +6528,28 @@
         <v>24</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P5" s="24" t="s">
         <v>68</v>
@@ -6565,7 +6574,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y5" s="9">
         <v>0</v>
@@ -6580,7 +6589,7 @@
         <v>68</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD5" s="14">
         <v>200</v>
@@ -6594,19 +6603,19 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:32">
       <c r="A6" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>23</v>
@@ -6615,28 +6624,28 @@
         <v>24</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P6" s="24" t="s">
         <v>68</v>
@@ -6661,7 +6670,7 @@
         <v>400000</v>
       </c>
       <c r="X6" s="24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Y6" s="9">
         <v>0</v>
@@ -6676,7 +6685,7 @@
         <v>68</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AD6" s="14">
         <v>200</v>
@@ -6756,124 +6765,124 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="Y1" s="18" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="Z1" s="19" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="AA1" s="19" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="AB1" s="19" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="AC1" s="19" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="AD1" s="19" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="AE1" s="19" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="AF1" s="19" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="AG1" s="19" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="AH1" s="19" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="AI1" s="19" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AJ1" s="19" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AK1" s="19" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AL1" s="19" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AM1" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AN1" s="19" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="AO1" s="19" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="AP1" s="18" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="AQ1" s="18" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="AR1" s="20" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="AS1" s="10" t="s">
         <v>9</v>
@@ -6882,37 +6891,37 @@
         <v>10</v>
       </c>
       <c r="AU1" s="12" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:47">
       <c r="A2" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K2" s="5">
         <v>1600000</v>
@@ -6924,34 +6933,34 @@
         <v>1600000</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Q2" s="5">
         <v>0</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="V2" s="5">
         <v>0</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
@@ -6967,25 +6976,25 @@
       <c r="AK2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AM2" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AN2" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AO2" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AP2" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AR2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="AS2" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="AT2" s="14">
         <v>200</v>
@@ -6996,32 +7005,32 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:47">
       <c r="A3" s="5" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K3" s="5">
         <v>8800000</v>
@@ -7033,34 +7042,34 @@
         <v>1600000</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Q3" s="5">
         <v>0</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="V3" s="5">
         <v>0</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -7076,25 +7085,25 @@
       <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AM3" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AN3" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AO3" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AP3" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AQ3" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AR3" s="21" t="s">
         <v>68</v>
       </c>
       <c r="AS3" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="AT3" s="14">
         <v>200</v>
@@ -7105,32 +7114,32 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:47">
       <c r="A4" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K4" s="5">
         <v>1600000</v>
@@ -7142,34 +7151,34 @@
         <v>1600000</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Q4" s="5">
         <v>0</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="V4" s="5">
         <v>0</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
@@ -7185,25 +7194,25 @@
       <c r="AK4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AM4" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AN4" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AO4" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AP4" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AQ4" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AR4" s="21" t="s">
         <v>68</v>
       </c>
       <c r="AS4" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="AT4" s="14">
         <v>200</v>
@@ -7214,32 +7223,32 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:47">
       <c r="A5" s="5" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K5" s="5">
         <v>1600000</v>
@@ -7251,34 +7260,34 @@
         <v>1600000</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Q5" s="5">
         <v>0</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="V5" s="5">
         <v>0</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="X5" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -7294,25 +7303,25 @@
       <c r="AK5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AM5" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AN5" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AO5" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AP5" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AQ5" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AR5" s="21" t="s">
         <v>68</v>
       </c>
       <c r="AS5" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="AT5" s="14">
         <v>200</v>
@@ -7323,32 +7332,32 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:47">
       <c r="A6" s="5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K6" s="5">
         <v>1600000</v>
@@ -7360,34 +7369,34 @@
         <v>1600000</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Q6" s="5">
         <v>0</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="V6" s="5">
         <v>0</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
@@ -7403,25 +7412,25 @@
       <c r="AK6" s="5"/>
       <c r="AL6" s="5"/>
       <c r="AM6" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AN6" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AO6" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AP6" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AQ6" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AR6" s="21" t="s">
         <v>68</v>
       </c>
       <c r="AS6" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="AT6" s="14">
         <v>200</v>
@@ -7432,32 +7441,32 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="69" customHeight="1" spans="1:47">
       <c r="A7" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K7" s="5">
         <v>100000</v>
@@ -7469,90 +7478,90 @@
         <v>100000</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Q7" s="5">
         <v>0</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="V7" s="5">
         <v>0</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA7" s="5">
         <v>200000</v>
       </c>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="AD7" s="5"/>
       <c r="AE7" s="5">
         <v>200000</v>
       </c>
       <c r="AF7" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AG7" s="5">
         <v>0</v>
       </c>
       <c r="AH7" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="AI7" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="AL7" s="5">
         <v>0</v>
       </c>
       <c r="AM7" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AN7" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AO7" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="AP7" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AQ7" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AR7" s="21" t="s">
         <v>68</v>
       </c>
       <c r="AS7" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="AT7" s="14">
         <v>200</v>
@@ -7834,22 +7843,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>9</v>
@@ -7858,48 +7867,48 @@
         <v>10</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:19">
       <c r="A2" s="5" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>23</v>
@@ -7911,16 +7920,16 @@
         <v>26</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="L2" s="14">
         <v>200</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="O2" s="15"/>
       <c r="P2" s="5">
@@ -7932,25 +7941,25 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:19">
       <c r="A3" s="5" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>23</v>
@@ -7962,16 +7971,16 @@
         <v>26</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="L3" s="14">
         <v>200</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="5">
@@ -7983,25 +7992,25 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:19">
       <c r="A4" s="5" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>23</v>
@@ -8013,16 +8022,16 @@
         <v>26</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="L4" s="14">
         <v>200</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="O4" s="15"/>
       <c r="P4" s="5">
@@ -8034,25 +8043,25 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:19">
       <c r="A5" s="5" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>23</v>
@@ -8064,16 +8073,16 @@
         <v>26</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="L5" s="14">
         <v>200</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="5">
@@ -8085,25 +8094,25 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:19">
       <c r="A6" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>23</v>
@@ -8115,29 +8124,29 @@
         <v>26</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="L6" s="14">
         <v>200</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="5">
         <v>100000</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -8184,10 +8193,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>9</v>
@@ -8196,33 +8205,33 @@
         <v>10</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:10">
       <c r="A2" s="5" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="H2" s="14">
         <v>200</v>
@@ -8231,30 +8240,30 @@
         <v>31</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:10">
       <c r="A3" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="H3" s="14">
         <v>200</v>
@@ -8263,30 +8272,30 @@
         <v>31</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:10">
       <c r="A4" s="5" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="H4" s="14">
         <v>200</v>
@@ -8295,30 +8304,30 @@
         <v>31</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:10">
       <c r="A5" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="H5" s="14">
         <v>200</v>
@@ -8327,7 +8336,7 @@
         <v>31</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -8341,7 +8350,7 @@
   <sheetPr/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -8373,16 +8382,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>9</v>
@@ -8391,36 +8400,36 @@
         <v>10</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="69" customHeight="1" spans="1:11">
       <c r="A2" s="5" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="J2" s="14">
         <v>200</v>
@@ -8882,8 +8891,8 @@
   <sheetPr/>
   <dimension ref="A1:AL11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -9598,14 +9607,229 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" customHeight="1" spans="9:15">
-      <c r="I7" s="16"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="16"/>
+    <row r="7" s="1" customFormat="1" ht="52" customHeight="1" spans="1:38">
+      <c r="A7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="9">
+        <v>200</v>
+      </c>
+      <c r="L7" s="14">
+        <v>1800000</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>1800000</v>
+      </c>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14">
+        <v>1</v>
+      </c>
+      <c r="T7" s="14">
+        <v>800000</v>
+      </c>
+      <c r="U7" s="14">
+        <v>400000</v>
+      </c>
+      <c r="V7" s="14">
+        <v>200000</v>
+      </c>
+      <c r="W7" s="14">
+        <v>200000</v>
+      </c>
+      <c r="X7" s="14">
+        <v>800000</v>
+      </c>
+      <c r="Y7" s="14">
+        <v>400000</v>
+      </c>
+      <c r="Z7" s="14">
+        <v>1200000</v>
+      </c>
+      <c r="AA7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="14">
+        <v>800000</v>
+      </c>
+      <c r="AD7" s="14">
+        <v>1600000</v>
+      </c>
+      <c r="AE7" s="14">
+        <v>600000</v>
+      </c>
+      <c r="AF7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="14">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="52" customHeight="1" spans="1:38">
+      <c r="A8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="9">
+        <v>200</v>
+      </c>
+      <c r="L8" s="14">
+        <v>1200000</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>1200000</v>
+      </c>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14">
+        <v>1</v>
+      </c>
+      <c r="T8" s="14">
+        <v>800000</v>
+      </c>
+      <c r="U8" s="14">
+        <v>400000</v>
+      </c>
+      <c r="V8" s="14">
+        <v>200000</v>
+      </c>
+      <c r="W8" s="14">
+        <v>200000</v>
+      </c>
+      <c r="X8" s="14">
+        <v>800000</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>400000</v>
+      </c>
+      <c r="Z8" s="14">
+        <v>1200000</v>
+      </c>
+      <c r="AA8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="14">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="14">
+        <v>800000</v>
+      </c>
+      <c r="AD8" s="14">
+        <v>1200000</v>
+      </c>
+      <c r="AE8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="14">
+        <v>1200000</v>
+      </c>
     </row>
     <row r="11" customHeight="1" spans="12:12">
       <c r="L11" s="36"/>
@@ -10114,7 +10338,7 @@
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:38">
       <c r="A5" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>72</v>
@@ -11652,7 +11876,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>9</v>
@@ -11699,7 +11923,7 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:23">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>66</v>
@@ -11724,7 +11948,7 @@
         <v>68</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K2" s="9">
         <v>200</v>
@@ -11764,7 +11988,7 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:23">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>70</v>
@@ -11789,7 +12013,7 @@
         <v>68</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K3" s="9">
         <v>200</v>
@@ -11829,7 +12053,7 @@
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:23">
       <c r="A4" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>72</v>
@@ -11854,7 +12078,7 @@
         <v>68</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K4" s="9">
         <v>200</v>
@@ -11919,7 +12143,7 @@
         <v>68</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K5" s="9">
         <v>200</v>
@@ -11961,7 +12185,7 @@
     </row>
     <row r="6" s="1" customFormat="1" customHeight="1" spans="1:23">
       <c r="A6" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>76</v>
@@ -11986,7 +12210,7 @@
         <v>68</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K6" s="9">
         <v>200</v>

</xml_diff>